<commit_message>
add the getMethod test
</commit_message>
<xml_diff>
--- a/Testcase-query.xlsx
+++ b/Testcase-query.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BJgvoTestcase" sheetId="2" r:id="rId2"/>
+    <sheet name="TBphone" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>案例编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,6 +99,38 @@
   </si>
   <si>
     <t>是的热v热风我的份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京建造师发布平台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://bjjs.zjw.beijing.gov.cn/eportal/ui?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京市住房和城乡建设委员会门户网站</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +151,14 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -137,18 +179,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -452,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -572,4 +620,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="42.77734375" customWidth="1"/>
+    <col min="8" max="8" width="38.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4">
+        <v>314443</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1">
+        <v>314443</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>